<commit_message>
upto 239ed7 plus build files
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/eventsliders.xlsx
+++ b/doc/help_dialogs/Input_files/eventsliders.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="275">
   <si>
     <t xml:space="preserve">EVENT CUSTOM SLIDERS</t>
   </si>
@@ -59,7 +59,7 @@
     <t xml:space="preserve">Factor</t>
   </si>
   <si>
-    <t xml:space="preserve">Scale factor, Slider value is multplied by this value.</t>
+    <t xml:space="preserve">Scale factor, Slider value is multiplied by this value.</t>
   </si>
   <si>
     <t xml:space="preserve">Min</t>
@@ -95,10 +95,10 @@
     <t xml:space="preserve">COMMANDS</t>
   </si>
   <si>
-    <t xml:space="preserve">tn:Note: "{}" can be used as a placeholder, it will be subsituted by (value*factor + offset). In all slider command actions, but for IO, VOUT, S7 and RC Commands, the bound value is converted from a float to an int.\n</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tn:Note: The placeholders {ET}, {BT}, {time}, {ETB}, {BTB} will be substituted by the current ET, BT, time, ET background, BT background value in Serial/CallProgram/MODBUS/S7/WebSocket commands\n</t>
+    <t xml:space="preserve">tn:Note: "{}" can be used as a placeholder, it will be substituted by (value*factor + offset). In all slider command actions, but for IO, VOUT, S7 and RC Commands, the bound value is converted from a float to an int.\n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tn:Note: The placeholders {ET}, {BT}, {time}, {ETB}, {BTB}, and {WEIGHTin} will be substituted by the current ET, BT, time, ET background, BT background value, and batch size (in g) in Serial/Artisan/CallProgram/MODBUS/S7/WebSocket commands\n</t>
   </si>
   <si>
     <t xml:space="preserve">tn:Note: commands can be sequenced, separated by semicolons like in “&lt;cmd1&gt;;&lt;cmd2&gt;;&lt;cmd3&gt;”\n</t>
@@ -143,6 +143,42 @@
     <t xml:space="preserve">reads register from slave slaveID using function 3 (Read Multiple Holding Registers). The result is bound to the placeholder `_` and thus can be accessed in later commands.</t>
   </si>
   <si>
+    <t xml:space="preserve">readSigned(slaveId,register)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reads 1 16bit register from slave slaveID using function 3 (Read Multiple Holding Registers) interpreted as signed integer. The result is bound to the placeholder `_` and thus can be accessed in later commands.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">readBCD(slaveID,register)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reads 1 16bit register from slave slaveID using function 3 (Read Multiple Holding Registers) interpreted as BCD. The result is bound to the placeholder `_` and thus can be accessed in later commands.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">read32(slaveID,register)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reads 2 16bit registers from slave slaveID using function 3 (Read Multiple Holding Registers) interpreted as unsigned integer. The result is bound to the placeholder `_` and thus can be accessed in later commands.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">read32Signed(slaveID,register)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reads 2 16bit registers from slave slaveID using function 3 (Read Multiple Holding Registers) interpreted as signed integer. The result is bound to the placeholder `_` and thus can be accessed in later commands.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">read32BCD(slaveID,register)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reads 2 16bit register from slave slaveID using function 3 (Read Multiple Holding Registers) interpreted as BCD. The result is bound to the placeholder `_` and thus can be accessed in later commands.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">readFloat(slaveID,register)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reads 2 16bit registers from slave slaveID using function 3 (Read Multiple Holding Registers) interpreted as float. The result is bound to the placeholder `_` and thus can be accessed in later commands.</t>
+  </si>
+  <si>
     <t xml:space="preserve">write(slaveId,register,value) or write([slaveId,register,value],..,[slaveId,register,value])</t>
   </si>
   <si>
@@ -188,6 +224,12 @@
     <t xml:space="preserve">write 32bit float to two 16bit int registers: MODBUS function 16</t>
   </si>
   <si>
+    <t xml:space="preserve">writeLong(slaveId,register,value) or writeLong([slaveId,register,value],..,[slaveId,register,value])</t>
+  </si>
+  <si>
+    <t xml:space="preserve">write 32bit integer to two 16bit int registers: MODBUS function 16</t>
+  </si>
+  <si>
     <t xml:space="preserve">writeSingle(slaveId,register,value) or writeSingle([slaveId,register,value],..,[slaveId,register,value])</t>
   </si>
   <si>
@@ -308,7 +350,7 @@
     <t xml:space="preserve">range(c,r[,sn])</t>
   </si>
   <si>
-    <t xml:space="preserve">for PHIDGET OUTPUT modules: sets voltage voltage range (r=5 fo r5V and r=10 for 10V)</t>
+    <t xml:space="preserve">for PHIDGET OUTPUT modules: sets voltage voltage range (r=5 for r5V and r=10 for 10V)</t>
   </si>
   <si>
     <t xml:space="preserve">out(n,v[,sn])</t>
@@ -386,6 +428,12 @@
     <t xml:space="preserve">YOCTOPUCE Relay Output: turn channel c of the relay module off</t>
   </si>
   <si>
+    <t xml:space="preserve">yset(c,b[,sn])</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YOCTOPUCE Relay Output: switches channel c of the relay module off (b=0) and on (b=1)</t>
+  </si>
+  <si>
     <t xml:space="preserve">flip(c[,sn])</t>
   </si>
   <si>
@@ -398,6 +446,12 @@
     <t xml:space="preserve">YOCTOPUCE Relay Output: pulse the channel c on after a delay of delay milliseconds for the duration of duration milliseconds</t>
   </si>
   <si>
+    <t xml:space="preserve">powerReset([sn])</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YOCTOPUCE resets the power counter of the Yocto-Watt module</t>
+  </si>
+  <si>
     <t xml:space="preserve">slider(c,v)</t>
   </si>
   <si>
@@ -407,7 +461,37 @@
     <t xml:space="preserve">button(i,c,b[,sn])</t>
   </si>
   <si>
-    <t xml:space="preserve">switches channel c off (b=0) and on (b=1) and sets button i to pressed or normal depending on the value b</t>
+    <t xml:space="preserve">switches PHIDGET Binary Output channel c off (b=0) and on (b=1) and sets button i to pressed or normal depending on the value b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">button(i,b)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sets button i to pressed if value b is yes, true, t, or 1, otherwise to normal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">button(b)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sets button to pressed if value b is yes, true, t, or 1, otherwise to normal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">button()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggles the state of the button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">santoker(&lt;target&gt;,&lt;value&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sends integer &lt;value&gt; to &lt;target&gt; register specified by as byte in hex notation like “fa” via the Santoker Network protocol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kaleido(&lt;target&gt;,&lt;value&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sends &lt;value&gt; to &lt;target&gt; via the Kaleido Serial or Network protocol</t>
   </si>
   <si>
     <t xml:space="preserve">S7 Command</t>
@@ -536,6 +620,12 @@
     <t xml:space="preserve">sets the PID target set value SV</t>
   </si>
   <si>
+    <t xml:space="preserve">pidSVC(&lt;int&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sets the PID target set value SV given in C</t>
+  </si>
+  <si>
     <t xml:space="preserve">pidRS(&lt;rs&gt;)</t>
   </si>
   <si>
@@ -566,6 +656,18 @@
     <t xml:space="preserve">shows message &lt;msg&gt; in the message line</t>
   </si>
   <si>
+    <t xml:space="preserve">notifications(&lt;bool&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">enables/disables notifications; while disabled issued notifications are ignored</t>
+  </si>
+  <si>
+    <t xml:space="preserve">notify(&lt;title&gt;,[&lt;msg&gt;])</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sends notification with title &lt;title&gt; and optional message &lt;msg&gt;</t>
+  </si>
+  <si>
     <t xml:space="preserve">setCanvasColor(&lt;color&gt;)</t>
   </si>
   <si>
@@ -630,6 +732,36 @@
   </si>
   <si>
     <t xml:space="preserve">enables/disables keyboard mode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">keepON(&lt;bool&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">enables/disables the Keep ON flag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">showCurve(&lt;name&gt;,&lt;bool&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shows/hides the curve indicated by &lt;name&gt; which is one of { ET, BT, DeltaET, DeltaBT, BackgroundET, BackgroundBT}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">showExtraCurve(&lt;extra_device&gt;,&lt;curve&gt;,&lt;bool&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shows/hides the &lt;curve&gt; (one of {T1,T2}) of the zero-based &lt;extra_device&gt; number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">showEvents(&lt;event_type&gt;, &lt;bool&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shows/hides the events of &lt;event_type&gt; in [1,..,5]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">showBackgroundEvents(&lt;bool&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shows/hides the events of the background profile</t>
   </si>
   <si>
     <t xml:space="preserve">RC Command</t>
@@ -723,7 +855,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -745,6 +877,14 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -789,7 +929,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -798,7 +938,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -822,10 +970,10 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="1" sqref="95:95 B6"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.78515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.03125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="70.31"/>
@@ -940,15 +1088,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C111"/>
+  <dimension ref="A1:C133"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A85" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A95" activeCellId="0" sqref="95:95"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.78515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.03125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.57"/>
   </cols>
   <sheetData>
@@ -1005,7 +1153,7 @@
       <c r="A9" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="2" t="s">
         <v>32</v>
       </c>
       <c r="C9" s="0" t="s">
@@ -1013,7 +1161,7 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="2" t="s">
         <v>34</v>
       </c>
       <c r="C10" s="0" t="s">
@@ -1021,7 +1169,7 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="2" t="s">
         <v>36</v>
       </c>
       <c r="C11" s="0" t="s">
@@ -1029,15 +1177,15 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="2" t="s">
         <v>38</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="1" t="s">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="2" t="s">
         <v>40</v>
       </c>
       <c r="C13" s="0" t="s">
@@ -1045,7 +1193,7 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C14" s="0" t="s">
@@ -1053,7 +1201,7 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="0" t="s">
+      <c r="B15" s="2" t="s">
         <v>44</v>
       </c>
       <c r="C15" s="0" t="s">
@@ -1061,182 +1209,182 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="B16" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="C16" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="C16" s="0" t="s">
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="2" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="0" t="s">
+      <c r="C17" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="C17" s="0" t="s">
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="0" t="s">
+      <c r="C18" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="C18" s="0" t="s">
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="2" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="19" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="0" t="s">
+      <c r="C19" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="C19" s="0" t="s">
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="20" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="0" t="s">
+      <c r="C20" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="C20" s="0" t="s">
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="21" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+      <c r="C21" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="B21" s="2" t="s">
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="C21" s="0" t="s">
+      <c r="B22" s="2" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+      <c r="C22" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="B22" s="0" t="s">
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C22" s="0" t="s">
+      <c r="C23" s="0" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C23" s="0" t="s">
+      <c r="C24" s="0" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C24" s="0" t="s">
+      <c r="C25" s="0" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="C26" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="C25" s="0" t="s">
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="2" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+      <c r="C27" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="B26" s="0" t="s">
+    </row>
+    <row r="28" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
+      <c r="B28" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B27" s="0" t="s">
+      <c r="C28" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="C27" s="0" t="s">
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="0" t="s">
+      <c r="B29" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="C28" s="0" t="s">
+      <c r="C29" s="0" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="0" t="s">
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="C29" s="0" t="s">
+      <c r="C30" s="0" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="0" t="s">
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
         <v>79</v>
       </c>
-      <c r="C30" s="0" t="s">
+      <c r="C31" s="0" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="0" t="s">
+    <row r="32" customFormat="false" ht="28.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="C31" s="0" t="s">
+      <c r="B32" s="4" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="0" t="s">
+      <c r="C32" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="C32" s="0" t="s">
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="0" t="s">
+      <c r="B33" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C33" s="0" t="s">
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="0" t="s">
+      <c r="B34" s="2" t="s">
         <v>87</v>
       </c>
       <c r="C34" s="0" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="0" t="s">
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="2" t="s">
         <v>89</v>
       </c>
       <c r="C35" s="0" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="0" t="s">
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="2" t="s">
         <v>91</v>
       </c>
       <c r="C36" s="0" t="s">
@@ -1244,418 +1392,421 @@
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
+      <c r="B37" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B37" s="0" t="s">
+      <c r="C37" s="0" t="s">
         <v>94</v>
       </c>
-      <c r="C37" s="0" t="s">
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="2" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="0" t="s">
+      <c r="C38" s="0" t="s">
         <v>96</v>
       </c>
-      <c r="C38" s="0" t="s">
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="2" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="0" t="s">
+      <c r="C39" s="0" t="s">
         <v>98</v>
       </c>
-      <c r="C39" s="0" t="s">
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="2" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="0" t="s">
+      <c r="C40" s="0" t="s">
         <v>100</v>
       </c>
-      <c r="C40" s="0" t="s">
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B41" s="2" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="0" t="s">
-        <v>34</v>
-      </c>
       <c r="C41" s="0" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="B42" s="0" t="s">
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B42" s="2" t="s">
         <v>103</v>
       </c>
       <c r="C42" s="0" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="0" t="s">
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B43" s="2" t="s">
         <v>105</v>
       </c>
       <c r="C43" s="0" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="0" t="s">
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
         <v>107</v>
       </c>
+      <c r="B44" s="2" t="s">
+        <v>108</v>
+      </c>
       <c r="C44" s="0" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="0" t="s">
         <v>109</v>
       </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B45" s="2" t="s">
+        <v>110</v>
+      </c>
       <c r="C45" s="0" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="0" t="s">
         <v>111</v>
       </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B46" s="2" t="s">
+        <v>112</v>
+      </c>
       <c r="C46" s="0" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="0" t="s">
         <v>113</v>
       </c>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B47" s="2" t="s">
+        <v>114</v>
+      </c>
       <c r="C47" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B48" s="1" t="s">
-        <v>115</v>
+      <c r="B48" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="C48" s="0" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B49" s="0" t="s">
+      <c r="B49" s="2" t="s">
         <v>117</v>
       </c>
       <c r="C49" s="0" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B50" s="0" t="s">
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B50" s="2" t="s">
         <v>119</v>
       </c>
       <c r="C50" s="0" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B51" s="0" t="s">
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B51" s="2" t="s">
         <v>121</v>
       </c>
       <c r="C51" s="0" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B52" s="0" t="s">
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B52" s="2" t="s">
         <v>123</v>
       </c>
       <c r="C52" s="0" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B53" s="0" t="s">
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B53" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C53" s="0" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B54" s="0" t="s">
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B54" s="2" t="s">
         <v>127</v>
       </c>
       <c r="C54" s="0" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B55" s="0" t="s">
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B55" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C55" s="0" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B56" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C56" s="0" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B57" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C57" s="0" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B58" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C58" s="0" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B59" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C59" s="0" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B60" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C60" s="0" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B61" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C61" s="0" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B62" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C62" s="0" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B63" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="C63" s="0" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B64" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B65" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C65" s="0" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B66" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C66" s="0" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B67" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C55" s="0" t="s">
+      <c r="C67" s="0" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="B56" s="1" t="s">
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B68" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C68" s="0" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B69" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C69" s="0" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B70" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C56" s="1" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="1"/>
-      <c r="B57" s="1" t="s">
+      <c r="C70" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="1"/>
+      <c r="B71" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C57" s="1" t="s">
+      <c r="C71" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="1"/>
-      <c r="B58" s="0" t="s">
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="1"/>
+      <c r="B72" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C58" s="0" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B59" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="1"/>
-      <c r="B60" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="1"/>
-      <c r="B61" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="1"/>
-      <c r="B62" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="1"/>
-      <c r="B63" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="1"/>
-      <c r="B64" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="0" t="s">
-        <v>144</v>
-      </c>
-      <c r="C65" s="0" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="0" t="s">
-        <v>145</v>
-      </c>
-      <c r="C66" s="0" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="0" t="s">
-        <v>146</v>
-      </c>
-      <c r="C67" s="0" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="B68" s="0" t="s">
-        <v>149</v>
-      </c>
-      <c r="C68" s="0" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B69" s="0" t="s">
-        <v>151</v>
-      </c>
-      <c r="C69" s="0" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B70" s="0" t="s">
-        <v>153</v>
-      </c>
-      <c r="C70" s="0" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B71" s="0" t="s">
+      <c r="C72" s="0" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B73" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="1"/>
+      <c r="B74" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="1"/>
+      <c r="B75" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="1"/>
+      <c r="B76" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="1"/>
+      <c r="B77" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="1"/>
+      <c r="B78" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="B79" s="2"/>
+      <c r="C79" s="0" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="B80" s="2"/>
+      <c r="C80" s="0" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="B81" s="2"/>
+      <c r="C81" s="0" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C82" s="0" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B83" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="C83" s="0" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B84" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="C84" s="0" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B85" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C71" s="0" t="s">
+      <c r="C85" s="0" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B72" s="0" t="s">
-        <v>155</v>
-      </c>
-      <c r="C72" s="0" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B73" s="0" t="s">
-        <v>157</v>
-      </c>
-      <c r="C73" s="0" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B74" s="0" t="s">
-        <v>159</v>
-      </c>
-      <c r="C74" s="0" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B75" s="0" t="s">
-        <v>161</v>
-      </c>
-      <c r="C75" s="0" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B76" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="C76" s="0" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B77" s="0" t="s">
-        <v>165</v>
-      </c>
-      <c r="C77" s="0" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B78" s="0" t="s">
-        <v>167</v>
-      </c>
-      <c r="C78" s="0" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B79" s="0" t="s">
-        <v>169</v>
-      </c>
-      <c r="C79" s="0" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B80" s="0" t="s">
-        <v>171</v>
-      </c>
-      <c r="C80" s="0" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B81" s="0" t="s">
-        <v>173</v>
-      </c>
-      <c r="C81" s="0" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B82" s="0" t="s">
-        <v>175</v>
-      </c>
-      <c r="C82" s="0" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B83" s="0" t="s">
-        <v>177</v>
-      </c>
-      <c r="C83" s="0" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B84" s="0" t="s">
-        <v>179</v>
-      </c>
-      <c r="C84" s="0" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B85" s="0" t="s">
-        <v>181</v>
-      </c>
-      <c r="C85" s="0" t="s">
-        <v>182</v>
-      </c>
-    </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B86" s="0" t="s">
+      <c r="B86" s="2" t="s">
         <v>183</v>
       </c>
       <c r="C86" s="0" t="s">
@@ -1663,7 +1814,7 @@
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B87" s="0" t="s">
+      <c r="B87" s="2" t="s">
         <v>185</v>
       </c>
       <c r="C87" s="0" t="s">
@@ -1671,23 +1822,23 @@
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B88" s="0" t="s">
+      <c r="B88" s="2" t="s">
         <v>187</v>
       </c>
       <c r="C88" s="0" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B89" s="0" t="s">
+    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B89" s="2" t="s">
         <v>189</v>
       </c>
       <c r="C89" s="0" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B90" s="0" t="s">
+    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B90" s="2" t="s">
         <v>191</v>
       </c>
       <c r="C90" s="0" t="s">
@@ -1695,7 +1846,7 @@
       </c>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B91" s="0" t="s">
+      <c r="B91" s="2" t="s">
         <v>193</v>
       </c>
       <c r="C91" s="0" t="s">
@@ -1703,7 +1854,7 @@
       </c>
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B92" s="0" t="s">
+      <c r="B92" s="2" t="s">
         <v>195</v>
       </c>
       <c r="C92" s="0" t="s">
@@ -1711,7 +1862,7 @@
       </c>
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B93" s="0" t="s">
+      <c r="B93" s="2" t="s">
         <v>197</v>
       </c>
       <c r="C93" s="0" t="s">
@@ -1719,7 +1870,7 @@
       </c>
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B94" s="0" t="s">
+      <c r="B94" s="2" t="s">
         <v>199</v>
       </c>
       <c r="C94" s="0" t="s">
@@ -1727,117 +1878,111 @@
       </c>
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B95" s="0" t="s">
+      <c r="B95" s="2" t="s">
         <v>201</v>
       </c>
       <c r="C95" s="0" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="0" t="s">
+    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B96" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="B96" s="0" t="s">
+      <c r="C96" s="0" t="s">
         <v>204</v>
       </c>
-      <c r="C96" s="0" t="s">
+    </row>
+    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B97" s="2" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B97" s="0" t="s">
+      <c r="C97" s="0" t="s">
         <v>206</v>
       </c>
-      <c r="C97" s="0" t="s">
+    </row>
+    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B98" s="2" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B98" s="0" t="s">
+      <c r="C98" s="0" t="s">
         <v>208</v>
       </c>
-      <c r="C98" s="0" t="s">
+    </row>
+    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B99" s="2" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B99" s="0" t="s">
+      <c r="C99" s="0" t="s">
         <v>210</v>
       </c>
-      <c r="C99" s="0" t="s">
+    </row>
+    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B100" s="2" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B100" s="0" t="s">
+      <c r="C100" s="0" t="s">
         <v>212</v>
       </c>
-      <c r="C100" s="0" t="s">
+    </row>
+    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B101" s="2" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B101" s="0" t="s">
+      <c r="C101" s="0" t="s">
         <v>214</v>
       </c>
-      <c r="C101" s="0" t="s">
+    </row>
+    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B102" s="2" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B102" s="0" t="s">
+      <c r="C102" s="0" t="s">
         <v>216</v>
       </c>
-      <c r="C102" s="0" t="s">
+    </row>
+    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B103" s="2" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B103" s="0" t="s">
+      <c r="C103" s="0" t="s">
         <v>218</v>
       </c>
-      <c r="C103" s="0" t="s">
+    </row>
+    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B104" s="2" t="s">
         <v>219</v>
-      </c>
-    </row>
-    <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B104" s="0" t="s">
-        <v>85</v>
       </c>
       <c r="C104" s="0" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B105" s="0" t="s">
+    <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B105" s="2" t="s">
         <v>221</v>
       </c>
       <c r="C105" s="0" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B106" s="0" t="s">
+    <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B106" s="2" t="s">
         <v>223</v>
       </c>
       <c r="C106" s="0" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B107" s="0" t="s">
-        <v>94</v>
+    <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B107" s="2" t="s">
+        <v>225</v>
       </c>
       <c r="C107" s="0" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="0" t="s">
-        <v>226</v>
-      </c>
-      <c r="B108" s="0" t="s">
+      <c r="B108" s="2" t="s">
         <v>227</v>
       </c>
       <c r="C108" s="0" t="s">
@@ -1845,27 +1990,209 @@
       </c>
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B109" s="0" t="s">
+      <c r="B109" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="C109" s="0" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B110" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="C110" s="0" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B111" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="C111" s="0" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B112" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="C112" s="0" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B113" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="C113" s="0" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B114" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="C114" s="0" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B115" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="C115" s="0" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B116" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="C116" s="0" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B117" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="C117" s="0" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="0" t="s">
+        <v>247</v>
+      </c>
+      <c r="B118" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="C118" s="0" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B119" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="C119" s="0" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B120" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="C120" s="0" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B121" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="C121" s="0" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B122" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="C122" s="0" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B123" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="C123" s="0" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B124" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="C124" s="0" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B125" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="C125" s="0" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B126" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C126" s="0" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B127" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="C127" s="0" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B128" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="C128" s="0" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B129" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C129" s="0" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A130" s="0" t="s">
+        <v>270</v>
+      </c>
+      <c r="B130" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="C130" s="0" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B131" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C109" s="0" t="s">
+      <c r="C131" s="0" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B110" s="0" t="s">
+    <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B132" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C110" s="0" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B111" s="0" t="s">
-        <v>229</v>
-      </c>
-      <c r="C111" s="0" t="s">
-        <v>230</v>
+      <c r="C132" s="0" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B133" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="C133" s="0" t="s">
+        <v>274</v>
       </c>
     </row>
   </sheetData>

</xml_diff>